<commit_message>
after debug problem on tables in app. (1)-GUI updates.(2)-cancel oven read temp becouse its stuck the calibration proccess.
</commit_message>
<xml_diff>
--- a/test_config.xlsx
+++ b/test_config.xlsx
@@ -659,7 +659,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +757,7 @@
         <v>25.6</v>
       </c>
       <c r="I7" s="5">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>4</v>
@@ -773,20 +773,26 @@
       <c r="H8" s="14">
         <v>28</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
       <c r="K8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="L8" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G9" s="4">
         <v>0.7</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="14">
+        <v>30</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1</v>
+      </c>
       <c r="K9" s="12" t="s">
         <v>6</v>
       </c>
@@ -798,26 +804,34 @@
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="5"/>
+      <c r="H10" s="14">
+        <v>31</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1</v>
+      </c>
       <c r="K10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="L10" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G11" s="4">
         <v>1.4</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="14">
+        <v>32</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1</v>
+      </c>
       <c r="K11" s="12" t="s">
         <v>10</v>
       </c>
       <c r="L11" s="5">
-        <v>8</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>